<commit_message>
chore: Update Icons.xlsx and VnsErp2025.csproj
- Update icon documentation
- Update project configuration
</commit_message>
<xml_diff>
--- a/VnsErp2025/Docs/Icons.xlsx
+++ b/VnsErp2025/Docs/Icons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\Workspaces\2025\VNS_ERP_2025_FINAL\VnsErp2025\VnsErp2025\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480BFBC4-3A01-42E8-B601-44F202D3A002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF63A7-1DA4-4BE4-9145-7D659F96F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,8 +242,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}" name="Table1" displayName="Table1" ref="A3:F17" totalsRowShown="0">
-  <autoFilter ref="A3:F17" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}" name="Table1" displayName="Table1" ref="A3:F43" totalsRowShown="0">
+  <autoFilter ref="A3:F43" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{40DFCB20-C3A8-47FB-864A-F92BABAAEE5E}" name="MODULE"/>
     <tableColumn id="5" xr3:uid="{094A95BA-F998-4986-8789-8E0127149204}" name="GUI"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="A13:C17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat(ui): Add inventory icons and integrate to main form
- Add inventory-related SVG icons (hardware, insurance, inventory, invoice, replacement, supplier)
- Update FormMain.Designer.cs with new ribbon items for inventory management
- Add resource definitions in Resources.Designer.cs and Resources.resx
- Update Icons.xlsx documentation
- Update VnsErp2025.csproj with new resource files
</commit_message>
<xml_diff>
--- a/VnsErp2025/Docs/Icons.xlsx
+++ b/VnsErp2025/Docs/Icons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\Workspaces\2025\VNS_ERP_2025_FINAL\VnsErp2025\VnsErp2025\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF63A7-1DA4-4BE4-9145-7D659F96F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8638C053-A1BF-4EE8-BF29-77D16C510F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>BẢNG DANH SÁCH CÁC ICON TRONG HỆ THỐNG</t>
   </si>
@@ -187,6 +187,114 @@
   </si>
   <si>
     <t>variant.svg</t>
+  </si>
+  <si>
+    <t>XuatNhapTonKhoRibbonPage</t>
+  </si>
+  <si>
+    <t>Xuất - Nhập - Tồn kho</t>
+  </si>
+  <si>
+    <t>inventory.png</t>
+  </si>
+  <si>
+    <t>NhapBaoHanhBarButtonItem</t>
+  </si>
+  <si>
+    <t>NhapKhoRibbonPageGroup</t>
+  </si>
+  <si>
+    <t>Nhập bảo hành</t>
+  </si>
+  <si>
+    <t>insurance.svg</t>
+  </si>
+  <si>
+    <t>replacement.svg</t>
+  </si>
+  <si>
+    <t>Nhập hàng thương mại</t>
+  </si>
+  <si>
+    <t>NhapHangThuongMaiBarButtonItem</t>
+  </si>
+  <si>
+    <t>NhapLuuChuyenKhoBarButtonItem</t>
+  </si>
+  <si>
+    <t>Nhập lưu chuyển kho</t>
+  </si>
+  <si>
+    <t>supplier.svg</t>
+  </si>
+  <si>
+    <t>NhapNoiBoBarButtonItem</t>
+  </si>
+  <si>
+    <t>Nhập nội bộ</t>
+  </si>
+  <si>
+    <t>inventory (1).svg</t>
+  </si>
+  <si>
+    <t>NhapThietBiMuonBarButtonItem</t>
+  </si>
+  <si>
+    <t>Nhập thiết bị mượn - thuê</t>
+  </si>
+  <si>
+    <t>hardware.svg</t>
+  </si>
+  <si>
+    <t>XuatBaoHanhBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất hàng bảo hành</t>
+  </si>
+  <si>
+    <t>XuatHangThuongMaiBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất hàng thương mại</t>
+  </si>
+  <si>
+    <t>XuatLuuChuyenKhoBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất lưu chuyển kho</t>
+  </si>
+  <si>
+    <t>XuatNoiBoBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất nội bộ</t>
+  </si>
+  <si>
+    <t>XuatChoThueMuonBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất thiết bị mượn - thuê</t>
+  </si>
+  <si>
+    <t>XuatKhoRibbonPageGroup</t>
+  </si>
+  <si>
+    <t>StockInOutMasterHistoryBarButtonItem</t>
+  </si>
+  <si>
+    <t>StockInOutRibbonPageGroup</t>
+  </si>
+  <si>
+    <t>Phiếu xuất kho</t>
+  </si>
+  <si>
+    <t>invoice.svg</t>
+  </si>
+  <si>
+    <t>StockInOutProductHistoryBarButtonItem</t>
+  </si>
+  <si>
+    <t>Sản phẩm - dịch vụ</t>
   </si>
 </sst>
 </file>
@@ -519,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,6 +947,251 @@
         <v>53</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
feat(Inventory,FormMain): Add assembly export menu and enhance UI
- FormMain: Add menu item for Xuất Hàng Lắp Ráp (Assembly Export)
- FormMain.Designer: Enhanced toolbar with assembly export functionality
- DeviceBll, WarrantyBll: Complete namespace block structure
- Inventory.csproj: Updated project references
- Resources: Added dashboard.svg icon asset
- VnsErp2025.csproj: Updated resource references
- Icons.xlsx: Updated with assembly export icons
</commit_message>
<xml_diff>
--- a/VnsErp2025/Docs/Icons.xlsx
+++ b/VnsErp2025/Docs/Icons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\Workspaces\2025\VNS_ERP_2025_FINAL\VnsErp2025\VnsErp2025\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8638C053-A1BF-4EE8-BF29-77D16C510F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352B6EA9-B4A8-42AA-BACE-A74EB155CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-7515" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
   <si>
     <t>BẢNG DANH SÁCH CÁC ICON TRONG HỆ THỐNG</t>
   </si>
@@ -295,6 +295,15 @@
   </si>
   <si>
     <t>Sản phẩm - dịch vụ</t>
+  </si>
+  <si>
+    <t>XuatLapRapBarButtonItem</t>
+  </si>
+  <si>
+    <t>Xuất lắp ráp</t>
+  </si>
+  <si>
+    <t>dashboard.svg</t>
   </si>
 </sst>
 </file>
@@ -627,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,6 +1177,12 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
       <c r="C29" t="s">
         <v>85</v>
       </c>
@@ -1182,6 +1197,15 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
       <c r="D30" t="s">
         <v>88</v>
       </c>
@@ -1190,6 +1214,26 @@
       </c>
       <c r="F30" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add attribute migrations and version UI updates
</commit_message>
<xml_diff>
--- a/VnsErp2025/Docs/Icons.xlsx
+++ b/VnsErp2025/Docs/Icons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\Workspaces\2025\VNS_ERP_2025_FINAL\VnsErp2025\VnsErp2025\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352B6EA9-B4A8-42AA-BACE-A74EB155CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63481C-70F3-4B44-9F3C-8B1683E9ECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-7515" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
   <si>
     <t>BẢNG DANH SÁCH CÁC ICON TRONG HỆ THỐNG</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>dashboard.svg</t>
+  </si>
+  <si>
+    <t>AttributeBarButtonItem</t>
+  </si>
+  <si>
+    <t>Thuộc tính biến thể</t>
+  </si>
+  <si>
+    <t>data-classification.svg</t>
   </si>
 </sst>
 </file>
@@ -636,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,6 +1245,26 @@
         <v>92</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
feat: Integrate identifier scanner into XuatNoiBo and update main UI assets
Changes in XuatNoiBo (Internal Transfer):
- FrmXuatNoiBo.cs: Add identifier dialog launcher and result handler
- FrmXuatNoiBo.Designer.cs: Layout and control improvements
- UcXuatNoiBoDetail.cs: Add scanner button, auto-fill StockOutQty, show identifiers in GhiChu

Main app updates:
- FormMain.cs/Designer: Wire up menu/tool to launch identifier-enabled flows
- Program.cs: Update debug launcher
- Resources: Add insertimage.svg, update resources designer and resx
- VnsErp2025.csproj: Include new resource

Overall:
- Consistent identifier scanning UX across all stock out workflows
- Updated icons/assets for UI
</commit_message>
<xml_diff>
--- a/VnsErp2025/Docs/Icons.xlsx
+++ b/VnsErp2025/Docs/Icons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\Workspaces\2025\VNS_ERP_2025_FINAL\VnsErp2025\VnsErp2025\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A63481C-70F3-4B44-9F3C-8B1683E9ECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05478792-3613-45CE-B74C-EE41F09740B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-7515" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
   <si>
     <t>BẢNG DANH SÁCH CÁC ICON TRONG HỆ THỐNG</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>data-classification.svg</t>
+  </si>
+  <si>
+    <t>DinhDanhSpHhBarButtonItem</t>
+  </si>
+  <si>
+    <t>Định danh SPHH</t>
   </si>
 </sst>
 </file>
@@ -370,6 +376,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}" name="Table1" displayName="Table1" ref="A3:F43" totalsRowShown="0">
   <autoFilter ref="A3:F43" xr:uid="{44B94CB1-26DD-405F-A542-4E8A9DFD286C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F33">
+    <sortCondition ref="C3:C43"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{40DFCB20-C3A8-47FB-864A-F92BABAAEE5E}" name="MODULE"/>
     <tableColumn id="5" xr3:uid="{094A95BA-F998-4986-8789-8E0127149204}" name="GUI"/>
@@ -645,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B32"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,16 +702,16 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,16 +722,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -733,16 +742,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -753,16 +762,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,13 +785,13 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -793,16 +802,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,16 +822,16 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,16 +842,16 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,16 +862,16 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,16 +882,16 @@
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,16 +902,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -913,16 +922,16 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -933,16 +942,16 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -953,16 +962,16 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -973,16 +982,16 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,16 +1002,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1013,16 +1022,16 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1033,16 +1042,16 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1053,16 +1062,16 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1073,16 +1082,16 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,16 +1102,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1113,16 +1122,16 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1136,13 +1145,13 @@
         <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1156,13 +1165,13 @@
         <v>83</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1176,13 +1185,13 @@
         <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,16 +1202,16 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1213,16 +1222,16 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1253,16 +1262,36 @@
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E32" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>